<commit_message>
Dry Run Fix 3
</commit_message>
<xml_diff>
--- a/assets/puzzles/mala_stalls/menu.xlsx
+++ b/assets/puzzles/mala_stalls/menu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\hunt\assets\puzzles\mala_stalls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4D4BFFD-A56A-47B3-B76B-8EEAD1D20BEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE8E554-B416-466F-88A4-8FF4C1985D6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{53B32976-5706-43A2-B970-686CEAD5075E}"/>
   </bookViews>
@@ -780,7 +780,9 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1032,7 +1034,7 @@
         <v>48</v>
       </c>
       <c r="H10" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>47</v>
@@ -1086,7 +1088,7 @@
         <v>40</v>
       </c>
       <c r="H12" s="10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>39</v>
@@ -1113,7 +1115,7 @@
         <v>36</v>
       </c>
       <c r="H13" s="10">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>35</v>
@@ -1142,7 +1144,7 @@
         <v>32</v>
       </c>
       <c r="H14" s="11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Fixed puzzle issues raised during dry run
</commit_message>
<xml_diff>
--- a/assets/puzzles/mala_stalls/menu.xlsx
+++ b/assets/puzzles/mala_stalls/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\hunt\assets\puzzles\mala_stalls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE8E554-B416-466F-88A4-8FF4C1985D6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7994D036-0FB4-472A-A653-F191FAA3E98D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{53B32976-5706-43A2-B970-686CEAD5075E}"/>
   </bookViews>
@@ -780,9 +780,7 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1034,7 +1032,7 @@
         <v>48</v>
       </c>
       <c r="H10" s="10">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>47</v>
@@ -1088,7 +1086,7 @@
         <v>40</v>
       </c>
       <c r="H12" s="10">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>39</v>
@@ -1115,7 +1113,7 @@
         <v>36</v>
       </c>
       <c r="H13" s="10">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>35</v>
@@ -1144,7 +1142,7 @@
         <v>32</v>
       </c>
       <c r="H14" s="11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>31</v>

</xml_diff>